<commit_message>
[Ankur] Other product_update code
</commit_message>
<xml_diff>
--- a/data/excel/OtherServices.xlsx
+++ b/data/excel/OtherServices.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ankur.Yadav\git\ProjectQuadlabs\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83338273-B307-4851-A8ED-856E122D78B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415ECCFB-0DC7-42CF-A316-774F46A90E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="70">
   <si>
     <t>TestCaseId</t>
   </si>
@@ -131,9 +132,6 @@
     <t>15-Jul-2024</t>
   </si>
   <si>
-    <t>22-Jul-2024</t>
-  </si>
-  <si>
     <t>StartDate</t>
   </si>
   <si>
@@ -167,18 +165,9 @@
     <t>ItineraryType</t>
   </si>
   <si>
-    <t>MoreProduct</t>
-  </si>
-  <si>
     <t>Test 1</t>
   </si>
   <si>
-    <t>Verify on other Product</t>
-  </si>
-  <si>
-    <t>Demo Test3</t>
-  </si>
-  <si>
     <t>Triptype</t>
   </si>
   <si>
@@ -213,13 +202,58 @@
   </si>
   <si>
     <t>DirectFlights</t>
+  </si>
+  <si>
+    <t>Flight</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>PolicyName</t>
+  </si>
+  <si>
+    <t>Business trip - QL Business policy</t>
+  </si>
+  <si>
+    <t>Verify on other Product-Flight(One Way).</t>
+  </si>
+  <si>
+    <t>Verify on other Product-Flight(Round trip).</t>
+  </si>
+  <si>
+    <t>Test 2</t>
+  </si>
+  <si>
+    <t>16-Jul-2024</t>
+  </si>
+  <si>
+    <t>17-Jul-2024</t>
+  </si>
+  <si>
+    <t>One Way</t>
+  </si>
+  <si>
+    <t>Economy</t>
+  </si>
+  <si>
+    <t>12-Jul-2024</t>
+  </si>
+  <si>
+    <t>18-Jul-2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flight Itinerary 1 </t>
+  </si>
+  <si>
+    <t>Flight Itinerary 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -242,6 +276,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -273,7 +313,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -296,6 +336,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -303,27 +356,12 @@
   </cellStyleXfs>
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -351,7 +389,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -635,293 +688,429 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF2"/>
+  <dimension ref="A1:AG3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AE21" sqref="AE21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="8"/>
-    <col min="8" max="8" width="28.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12" style="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12" style="8" customWidth="1"/>
-    <col min="19" max="19" width="40" style="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9" style="8" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.5703125" style="8" customWidth="1"/>
-    <col min="24" max="24" width="13.5703125" style="8" customWidth="1"/>
-    <col min="25" max="25" width="9.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.7109375" style="8" customWidth="1"/>
-    <col min="28" max="28" width="8.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="36" style="8" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="33" max="16384" width="9.140625" style="8"/>
+    <col min="1" max="1" width="14.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="3"/>
+    <col min="8" max="8" width="28.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.5703125" style="3" customWidth="1"/>
+    <col min="18" max="18" width="12" style="3" customWidth="1"/>
+    <col min="19" max="19" width="40" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.7109375" style="3" customWidth="1"/>
+    <col min="23" max="23" width="11.5703125" style="3" customWidth="1"/>
+    <col min="24" max="24" width="13.5703125" style="3" customWidth="1"/>
+    <col min="25" max="25" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="31.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.7109375" style="3" customWidth="1"/>
+    <col min="29" max="29" width="8.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="36" style="3" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.140625" customWidth="1"/>
+    <col min="34" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="S1" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="U1" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="V1" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="W1" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="X1" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y1" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z1" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA1" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB1" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC1" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD1" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE1" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF1" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG1" s="17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="10">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q2" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="R2" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="V1" s="1" t="s">
+      <c r="S2" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="T2" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="U2" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="V2" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W2" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="X1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y1" s="1" t="s">
+      <c r="X2" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y2" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z2" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA2" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB2" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC2" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD2" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="AC1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AD1" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="AE1" s="17" t="s">
+      <c r="AE2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF2" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG2" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="10">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q3" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="R3" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="S3" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="T3" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="U3" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="V3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="W3" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="X3" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="AF1" s="14" t="s">
+      <c r="Y3" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z3" s="11" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="2" spans="1:32" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="15">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="N2" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q2" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="R2" s="15" t="s">
+      <c r="AA3" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB3" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC3" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD3" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="S2" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="T2" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="U2" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="V2" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="W2" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="X2" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y2" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z2" s="16" t="s">
+      <c r="AE3" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF3" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG3" s="10" t="s">
         <v>56</v>
-      </c>
-      <c r="AB2" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC2" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="AD2" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="AE2" s="13" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="16">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{B5B8C174-68B4-4827-98ED-8ED98A51DD76}">
+  <phoneticPr fontId="4" type="noConversion"/>
+  <dataValidations count="18">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G3" xr:uid="{B5B8C174-68B4-4827-98ED-8ED98A51DD76}">
       <formula1>"Normal,SSO"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{E30AB6F3-BFBE-4A25-9367-0806E2162558}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H3" xr:uid="{E30AB6F3-BFBE-4A25-9367-0806E2162558}">
       <formula1>"//staging117/sbt,//preprod.quadlabs.net/sbt/#,test.quadlabs.net/sbt,tripsource.co.in/sbt/#,//test.quadlabs.net/SSO_Login"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2" xr:uid="{EC3B641E-2CD6-45BE-B447-1CB53C534645}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M3" xr:uid="{EC3B641E-2CD6-45BE-B447-1CB53C534645}">
       <formula1>"Shubham1,Shubham,rsudesh15,Saurabh,Laxmi,sachinkumar,Piyush,Ankur"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2" xr:uid="{47592FE9-9977-4B60-B79A-72FB9844ADD3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K3" xr:uid="{47592FE9-9977-4B60-B79A-72FB9844ADD3}">
       <formula1>"Saurabh,Prince Chaurasia,Gunjan Swain,Shubham,Laxmi Khanal,Sudesh Kumar,Piyush,Ankur,D Divaker S,Ankur Yadav,Sachin Kumar"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2" xr:uid="{ABE1A435-89EB-40A9-8C01-F3E70DF28D5A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L3" xr:uid="{ABE1A435-89EB-40A9-8C01-F3E70DF28D5A}">
       <formula1>"Administrator,Travel Arranger,Employee"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{F3E4CD88-0D4F-4422-BE67-D8CD386DF8E0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F3" xr:uid="{F3E4CD88-0D4F-4422-BE67-D8CD386DF8E0}">
       <formula1>"sbt,preprod117"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{731AD89B-78A1-48DB-8468-195CED300F65}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C3" xr:uid="{731AD89B-78A1-48DB-8468-195CED300F65}">
       <formula1>"Applied,NotApplied"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2" xr:uid="{00FA4C84-BA81-42E2-B63A-36553D8FB807}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O3" xr:uid="{00FA4C84-BA81-42E2-B63A-36553D8FB807}">
       <formula1>"Poonam_Corp,Amazon,Demo Corporate,Lux_Test_corp,Null"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{1C41A665-F2E7-4A53-B836-D68EB0BE17C7}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3" xr:uid="{1C41A665-F2E7-4A53-B836-D68EB0BE17C7}">
       <formula1>"1,2,3,4,5,6,7,8"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2" xr:uid="{63264B7D-1C9E-4339-85FF-A8B0E8AA293D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N3" xr:uid="{63264B7D-1C9E-4339-85FF-A8B0E8AA293D}">
       <formula1>"Laxmi@123,Admin@123,S21FUMK6JAPLBYO,Shubham@123,BAVYBXVY09FKGTY,Piyush@123,Ankur@123,DWUFR8WRAR6SL1M"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{AF38A68A-E57C-4AC8-BE46-F2A45CB12D9E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I3" xr:uid="{AF38A68A-E57C-4AC8-BE46-F2A45CB12D9E}">
       <formula1>"shekhar.singh@quadlabs.com,sachin.kumar@quadlabs.com,Laxmi.khanal@quadlabs.com,ayushi.shivhare@quadlabs.com,Vikrant.prajapati@quadlabs.com,ankit.singh@quadlabs.com"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2" xr:uid="{3042EA9A-00EF-413D-8BEB-6B7B1983DB2A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P3" xr:uid="{3042EA9A-00EF-413D-8BEB-6B7B1983DB2A}">
       <formula1>"Old,New"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X2" xr:uid="{23A29CAC-0052-4F90-A514-9B663EC690DC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X2:X3" xr:uid="{23A29CAC-0052-4F90-A514-9B663EC690DC}">
       <formula1>"Flight,Hotel,MoreProduct"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y2" xr:uid="{069EB86C-AB6A-45C9-ABB9-F175BF8BC22B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y2:Y3" xr:uid="{069EB86C-AB6A-45C9-ABB9-F175BF8BC22B}">
       <formula1>"Domestic,International"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z2" xr:uid="{FBA2FE36-8828-4CC4-8E5B-1A2EDF43CD7B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB2:AB3" xr:uid="{E8EF33F4-1525-4081-B172-FC5D6E3DA1C4}">
+      <formula1>"Economy,Business,First,Premium Economy"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG2:AG3" xr:uid="{38A161C8-1E28-4B50-BB05-C8629A391C97}">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z2:Z3" xr:uid="{076957C6-FA9B-4BA8-8DDA-90CC2F740A4C}">
+      <formula1>"Business trip - QL Business policy,Business trip  - Testing"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA2:AA3" xr:uid="{2DB5DEA4-D7BD-445C-821F-284F6CF26E75}">
       <formula1>"One Way,Round Trip"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA2" xr:uid="{E8EF33F4-1525-4081-B172-FC5D6E3DA1C4}">
-      <formula1>"Economy,Business,First,Premium Economy"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="N2" r:id="rId1" display="Admin@123" xr:uid="{C9E6C07A-0E49-4568-83B2-9926C9EDC8B7}"/>
     <hyperlink ref="I2" r:id="rId2" display="shekhar.singh@quadlabs.com" xr:uid="{13C25909-4798-4E23-81B5-29BAB65A7375}"/>
+    <hyperlink ref="N3" r:id="rId3" display="Admin@123" xr:uid="{3ACA97FD-B2B0-45F0-AB2C-75412ACC142E}"/>
+    <hyperlink ref="I3" r:id="rId4" display="shekhar.singh@quadlabs.com" xr:uid="{B1908DA2-2EA6-44F0-BDD5-4BF7D9C3403B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{485EECA2-C326-47E1-B33C-93CC32E19527}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[Shubham] code on Complex Itinerary Air
</commit_message>
<xml_diff>
--- a/data/excel/OtherServices.xlsx
+++ b/data/excel/OtherServices.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ankur.Yadav\git\ProjectQuadlabs\data\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shubham.Natkar\git\ProjectQuadlabs\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415ECCFB-0DC7-42CF-A316-774F46A90E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B59FC7-FCA2-4A8A-B417-D9A2197EFFE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="78">
   <si>
     <t>TestCaseId</t>
   </si>
@@ -247,6 +247,30 @@
   </si>
   <si>
     <t>Flight Itinerary 2</t>
+  </si>
+  <si>
+    <t>Automation Test 1</t>
+  </si>
+  <si>
+    <t>ProductsName</t>
+  </si>
+  <si>
+    <t>NoOfProducts</t>
+  </si>
+  <si>
+    <t>ComplexItineraryAir,HotelsOnRequest,SelfDriveCar,Forex,ChauffeurDrivenCar,Visa,Insurance,Bus,Rail</t>
+  </si>
+  <si>
+    <t>CAJourneyType</t>
+  </si>
+  <si>
+    <t>CAClass</t>
+  </si>
+  <si>
+    <t>CAOCode</t>
+  </si>
+  <si>
+    <t>CAOriginCity</t>
   </si>
 </sst>
 </file>
@@ -313,7 +337,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -349,12 +373,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -406,6 +441,34 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -690,8 +753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1105,12 +1168,311 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{485EECA2-C326-47E1-B33C-93CC32E19527}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AD20" sqref="AD20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.42578125" style="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="23"/>
+    <col min="5" max="5" width="28.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" style="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" style="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" style="23" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5703125" style="23" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="36" style="23" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="10.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.7109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.7109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.28515625" style="23" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="30.7109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.42578125" style="23" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="33.28515625" style="23" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.5703125" style="23" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="10.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="47" style="3" customWidth="1"/>
+    <col min="31" max="31" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="33.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q1" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="R1" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="S1" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="T1" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="U1" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="V1" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="W1" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="X1" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y1" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z1" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA1" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB1" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC1" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="AD1" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE1" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="AF1" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG1" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="AH1" s="24" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="M2" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="N2" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q2" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="R2" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="S2" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="T2" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="U2" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="V2" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="W2" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="X2" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y2" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z2" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA2" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB2" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC2">
+        <v>9</v>
+      </c>
+      <c r="AD2" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE2" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF2" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations disablePrompts="1" count="16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2" xr:uid="{DF4A688D-EAE1-44C4-A7BF-2441206560DF}">
+      <formula1>"One Way,Round Trip"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2" xr:uid="{C1983F1A-F21B-4E83-AC36-25F786ECE188}">
+      <formula1>"Business trip - QL Business policy,Business trip  - Testing"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB2" xr:uid="{C95F136A-C84B-4EFC-8F0A-C5E05E905915}">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2 AF2" xr:uid="{9202FC0C-BCA9-40FB-8FF8-A27DC37B6D25}">
+      <formula1>"Economy,Business,First,Premium Economy"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2" xr:uid="{5E1520F8-7AF4-409C-B5D6-919D7B2BA1F6}">
+      <formula1>"Domestic,International"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2" xr:uid="{3CF9D7CF-D256-48B2-8FDC-607D2BB763BA}">
+      <formula1>"Flight,Hotel,MoreProduct"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{6F3754F0-FEB5-4A74-A098-386619C330F2}">
+      <formula1>"shekhar.singh@quadlabs.com,sachin.kumar@quadlabs.com,Laxmi.khanal@quadlabs.com,ayushi.shivhare@quadlabs.com,Vikrant.prajapati@quadlabs.com,ankit.singh@quadlabs.com"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2" xr:uid="{B22660F1-1D7B-472C-B385-4498CEB0DA09}">
+      <formula1>"Laxmi@123,Admin@123,S21FUMK6JAPLBYO,Shubham@123,BAVYBXVY09FKGTY,Piyush@123,Ankur@123,DWUFR8WRAR6SL1M"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{116AEC81-F8D8-4985-98F0-6A7FFCE8C8D8}">
+      <formula1>"sbt,preprod117"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{60D09136-C750-4680-A34A-320457565344}">
+      <formula1>"Administrator,Travel Arranger,Employee"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{02472E1C-DC1C-4747-98BD-674732B68CC6}">
+      <formula1>"Saurabh,Prince Chaurasia,Gunjan Swain,Shubham,Laxmi Khanal,Sudesh Kumar,Piyush,Ankur,D Divaker S,Ankur Yadav,Sachin Kumar"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2" xr:uid="{0C998EC2-A7BD-4826-A679-6CAE65284F8A}">
+      <formula1>"Shubham1,Shubham,rsudesh15,Saurabh,Laxmi,sachinkumar,Piyush,Ankur"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{27C1FD54-4DE8-44B1-B330-CFC211150764}">
+      <formula1>"//staging117/sbt,//preprod.quadlabs.net/sbt/#,test.quadlabs.net/sbt,tripsource.co.in/sbt/#,//test.quadlabs.net/SSO_Login"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{14BBF75D-F3C0-4D66-9C5B-4BEB838B38A6}">
+      <formula1>"Normal,SSO"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC2" xr:uid="{222BD394-E544-4494-B737-94D45AE13ED2}">
+      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE2" xr:uid="{CAB9BF8E-74B9-4F1A-ADB8-274C852A9C91}">
+      <formula1>"One Way,Round Trip,MultiCity"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="K2" r:id="rId1" display="Admin@123" xr:uid="{2581EA54-2092-4681-AD4E-6F1A6F7272CD}"/>
+    <hyperlink ref="F2" r:id="rId2" display="shekhar.singh@quadlabs.com" xr:uid="{E59B4478-6F3E-4D02-B79B-8644A35B9D35}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[Shubham] Code on Visa
</commit_message>
<xml_diff>
--- a/data/excel/OtherServices.xlsx
+++ b/data/excel/OtherServices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shubham.Natkar\git\ProjectQuadlabs\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B59FC7-FCA2-4A8A-B417-D9A2197EFFE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{264EDC57-9D4D-45BD-B4AF-ECF2F45BB8F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="124">
   <si>
     <t>TestCaseId</t>
   </si>
@@ -249,9 +249,6 @@
     <t>Flight Itinerary 2</t>
   </si>
   <si>
-    <t>Automation Test 1</t>
-  </si>
-  <si>
     <t>ProductsName</t>
   </si>
   <si>
@@ -271,6 +268,147 @@
   </si>
   <si>
     <t>CAOriginCity</t>
+  </si>
+  <si>
+    <t>HRStarCategory</t>
+  </si>
+  <si>
+    <t>MoreProduct</t>
+  </si>
+  <si>
+    <t>SCPickTime</t>
+  </si>
+  <si>
+    <t>SCPickCode</t>
+  </si>
+  <si>
+    <t>SCPickLocation</t>
+  </si>
+  <si>
+    <t>SCDropCode</t>
+  </si>
+  <si>
+    <t>SCDropLocation</t>
+  </si>
+  <si>
+    <t>BOM</t>
+  </si>
+  <si>
+    <t>Mumbai, India - Mumbai - Airport (130022)</t>
+  </si>
+  <si>
+    <t>DEL</t>
+  </si>
+  <si>
+    <t>New Delhi, India - New Delhi - Airport (130043)</t>
+  </si>
+  <si>
+    <t>SCCarType</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>ForPerDiem</t>
+  </si>
+  <si>
+    <t>CDCPickTime</t>
+  </si>
+  <si>
+    <t>CDCPickCode</t>
+  </si>
+  <si>
+    <t>CDCPickLocation</t>
+  </si>
+  <si>
+    <t>CDCDropCode</t>
+  </si>
+  <si>
+    <t>CDCDropLocation</t>
+  </si>
+  <si>
+    <t>CDCCarType</t>
+  </si>
+  <si>
+    <t>CDCRequirement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sedan </t>
+  </si>
+  <si>
+    <t>Transfers</t>
+  </si>
+  <si>
+    <t>Bisht Travels [6683]</t>
+  </si>
+  <si>
+    <t>CDCSupplier</t>
+  </si>
+  <si>
+    <t>OPTypeVisa</t>
+  </si>
+  <si>
+    <t>Visitor</t>
+  </si>
+  <si>
+    <t>OPIPolicyType</t>
+  </si>
+  <si>
+    <t>Excluding USA</t>
+  </si>
+  <si>
+    <t>OPIValidVisa</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>OBusOrigin</t>
+  </si>
+  <si>
+    <t>OBJournneyType</t>
+  </si>
+  <si>
+    <t>OBusDestination</t>
+  </si>
+  <si>
+    <t>OBusBoardingPoint</t>
+  </si>
+  <si>
+    <t>BD123</t>
+  </si>
+  <si>
+    <t>ORJourneyType</t>
+  </si>
+  <si>
+    <t>OROriginCode</t>
+  </si>
+  <si>
+    <t>ORDestinationCode</t>
+  </si>
+  <si>
+    <t>OR123</t>
+  </si>
+  <si>
+    <t>OD123</t>
+  </si>
+  <si>
+    <t>ORGender</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>ORGovernmentId</t>
+  </si>
+  <si>
+    <t>Voter ID</t>
+  </si>
+  <si>
+    <t>12:30</t>
+  </si>
+  <si>
+    <t>Automation Test 8</t>
   </si>
 </sst>
 </file>
@@ -337,7 +475,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -373,23 +511,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -457,19 +584,23 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1168,49 +1299,76 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{485EECA2-C326-47E1-B33C-93CC32E19527}">
-  <dimension ref="A1:AH2"/>
+  <dimension ref="A1:BJ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AD20" sqref="AD20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.42578125" style="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" style="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="23"/>
-    <col min="5" max="5" width="28.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.42578125" style="23" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" style="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" style="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.42578125" style="23" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="36" style="23" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="10.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.7109375" style="23" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.7109375" style="23" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.28515625" style="23" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="30.7109375" style="23" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.42578125" style="23" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="33.28515625" style="23" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="10.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="36" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="47" style="3" customWidth="1"/>
     <col min="31" max="31" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="9" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="10" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="14.5703125" customWidth="1"/>
+    <col min="56" max="56" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="17" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -1250,71 +1408,155 @@
       <c r="M1" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="N1" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="O1" s="16" t="s">
+      <c r="O1" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="P1" s="16" t="s">
+      <c r="P1" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="Q1" s="16" t="s">
+      <c r="Q1" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="R1" s="16" t="s">
+      <c r="R1" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="S1" s="16" t="s">
+      <c r="S1" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="T1" s="16" t="s">
+      <c r="T1" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="U1" s="16" t="s">
+      <c r="U1" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="V1" s="16" t="s">
+      <c r="V1" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="W1" s="16" t="s">
+      <c r="W1" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="X1" s="16" t="s">
+      <c r="X1" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="Y1" s="16" t="s">
+      <c r="Y1" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="Z1" s="17" t="s">
+      <c r="Z1" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="AA1" s="17" t="s">
+      <c r="AA1" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="AB1" s="17" t="s">
+      <c r="AB1" s="24" t="s">
         <v>54</v>
       </c>
       <c r="AC1" s="24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AD1" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AE1" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="AF1" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="AF1" s="24" t="s">
+      <c r="AG1" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="AG1" s="24" t="s">
+      <c r="AH1" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="AH1" s="24" t="s">
+      <c r="AI1" s="24" t="s">
         <v>77</v>
       </c>
+      <c r="AJ1" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK1" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL1" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="AM1" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN1" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="AO1" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="AP1" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="AQ1" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="AR1" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="AS1" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="AT1" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="AU1" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="AV1" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="AW1" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="AX1" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="AY1" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="AZ1" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="BA1" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="BB1" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="BC1" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="BD1" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="BE1" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="BF1" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="BG1" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="BH1" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="BI1" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="BJ1" s="24" t="s">
+        <v>120</v>
+      </c>
     </row>
-    <row r="2" spans="1:34" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:62" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>61</v>
       </c>
@@ -1349,7 +1591,7 @@
         <v>26</v>
       </c>
       <c r="L2" s="20" t="s">
-        <v>70</v>
+        <v>123</v>
       </c>
       <c r="M2" s="20" t="s">
         <v>47</v>
@@ -1370,7 +1612,7 @@
         <v>36</v>
       </c>
       <c r="S2" s="20" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="T2" s="11" t="s">
         <v>46</v>
@@ -1399,34 +1641,118 @@
       <c r="AB2" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="AC2">
-        <v>9</v>
-      </c>
-      <c r="AD2" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="AE2" s="27" t="s">
+      <c r="AC2" s="26">
+        <v>5</v>
+      </c>
+      <c r="AD2" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE2" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="AF2" s="27" t="s">
+      <c r="AF2" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AG2" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AH2" s="26" t="s">
         <v>40</v>
+      </c>
+      <c r="AI2" s="26">
+        <v>1</v>
+      </c>
+      <c r="AJ2" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="AK2" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL2" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="AM2" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="AN2" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="AO2" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="AP2" s="26">
+        <v>1000</v>
+      </c>
+      <c r="AQ2" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="AR2" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="AS2" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="AT2" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="AU2" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="AV2" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="AW2" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="AX2" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="AY2" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="AZ2" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="BA2" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="BB2" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="BC2" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="BD2" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="BE2" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="BF2" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="BG2" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="BH2" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="BI2" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="BJ2" s="26" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="16">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2" xr:uid="{DF4A688D-EAE1-44C4-A7BF-2441206560DF}">
+  <dataValidations count="25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2 BE2:BF2" xr:uid="{DF4A688D-EAE1-44C4-A7BF-2441206560DF}">
       <formula1>"One Way,Round Trip"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2" xr:uid="{C1983F1A-F21B-4E83-AC36-25F786ECE188}">
       <formula1>"Business trip - QL Business policy,Business trip  - Testing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB2" xr:uid="{C95F136A-C84B-4EFC-8F0A-C5E05E905915}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB2 BA2" xr:uid="{C95F136A-C84B-4EFC-8F0A-C5E05E905915}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2 AF2" xr:uid="{9202FC0C-BCA9-40FB-8FF8-A27DC37B6D25}">
@@ -1467,6 +1793,33 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE2" xr:uid="{CAB9BF8E-74B9-4F1A-ADB8-274C852A9C91}">
       <formula1>"One Way,Round Trip,MultiCity"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI2" xr:uid="{072D0C7B-288B-4876-A047-183510734653}">
+      <formula1>"1,2,3,4,5"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO2" xr:uid="{B18970A4-F4BE-4D08-8C98-C9B68EEC4E30}">
+      <formula1>"Normal,Luxury"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AV2" xr:uid="{B7702C5C-9F49-4BB5-8E2F-60199DFB5DBC}">
+      <formula1>"Sedan ,SUV,Others"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AW2" xr:uid="{09F39DBE-21FB-423D-9E44-E411BC3E112B}">
+      <formula1>"Transfers,Local Use,Outstation,Others "</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AX2" xr:uid="{57AFCA4F-73C7-489F-87D7-3884F385DAFD}">
+      <formula1>"Bisht Travels [6683],Dilpreet.Singh [VBAll],Shaan_Test_Supplier [Shaan Quadlabs],Hertz Brazil [HZBR],Tourico [TOUR],AMERICAN AIRLINE [0012],MALAYSIA ARLN [232],Ashish [321],Hotel_Supplier [211287],Abacus Travels [555],GDS Travels [4567],Ashu Yadav [S007]"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AY2" xr:uid="{B1F3BC6F-9159-49FB-BC67-7917E01AC80B}">
+      <formula1>"Visitor,Tourist,Employment,Work Permit,Business,Student,Dependent,Work Permit Dependent,Family Visitor,Domestic Worker,Permanent Migration"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AZ2" xr:uid="{CF313994-AC25-49DA-957E-D0AE3F825E4E}">
+      <formula1>"Excluding USA,Including USA"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BI2" xr:uid="{63A68163-1655-4818-AD76-238E7E466689}">
+      <formula1>"Male,Female,Others"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BJ2" xr:uid="{B4F78EDE-58D7-4E2C-B20C-72BF7B0C5141}">
+      <formula1>"Voter ID,Passport,PAN Card,Driving License"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>

</xml_diff>

<commit_message>
[Shubham] Update code on Other product
</commit_message>
<xml_diff>
--- a/data/excel/OtherServices.xlsx
+++ b/data/excel/OtherServices.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shubham.Natkar\git\ProjectQuadlabs\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{264EDC57-9D4D-45BD-B4AF-ECF2F45BB8F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04196E24-660A-46DB-BC49-740865EB1EB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="150">
   <si>
     <t>TestCaseId</t>
   </si>
@@ -408,7 +410,85 @@
     <t>12:30</t>
   </si>
   <si>
-    <t>Automation Test 8</t>
+    <t>ComplexItineraryAir,HotelsOnRequest,SelfDriveCar,Forex,Visa,Insurance,Bus,Rail</t>
+  </si>
+  <si>
+    <t>OPINomineeName</t>
+  </si>
+  <si>
+    <t>OPIRelation</t>
+  </si>
+  <si>
+    <t>Shubham Natkar</t>
+  </si>
+  <si>
+    <t>Friend</t>
+  </si>
+  <si>
+    <t>Test 3</t>
+  </si>
+  <si>
+    <t>Test 4</t>
+  </si>
+  <si>
+    <t>Test 5</t>
+  </si>
+  <si>
+    <t>Pnq</t>
+  </si>
+  <si>
+    <t>Pune,India - Lohegaon (PNQ)</t>
+  </si>
+  <si>
+    <t>22-Jul-2024</t>
+  </si>
+  <si>
+    <t>25-Jul-2024</t>
+  </si>
+  <si>
+    <t>10-Jul-2024</t>
+  </si>
+  <si>
+    <t>HotelsOnRequest,SelfDriveCar,Insurance,Bus</t>
+  </si>
+  <si>
+    <t>ComplexItineraryAir,Forex,Visa,Insurance,Bus,Rail</t>
+  </si>
+  <si>
+    <t>Visa,Insurance</t>
+  </si>
+  <si>
+    <t>Visa,Insurance,Bus</t>
+  </si>
+  <si>
+    <t>Automation Test 28</t>
+  </si>
+  <si>
+    <t>Automation Test 29</t>
+  </si>
+  <si>
+    <t>Automation Test 30</t>
+  </si>
+  <si>
+    <t>Automation Test 31</t>
+  </si>
+  <si>
+    <t>Automation Test 32</t>
+  </si>
+  <si>
+    <t>Verify on Other services with adding 8 products.</t>
+  </si>
+  <si>
+    <t>Verify on Other services with adding 4 products.</t>
+  </si>
+  <si>
+    <t>Verify on Other services with adding 2 products.</t>
+  </si>
+  <si>
+    <t>Verify on Other services with adding 3 products.</t>
+  </si>
+  <si>
+    <t>Verify on Other services with adding 6 products.</t>
   </si>
 </sst>
 </file>
@@ -516,7 +596,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -601,6 +681,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -885,7 +971,7 @@
   <dimension ref="A1:AG3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1299,16 +1385,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{485EECA2-C326-47E1-B33C-93CC32E19527}">
-  <dimension ref="A1:BJ2"/>
+  <dimension ref="A1:BL6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.42578125" bestFit="1" customWidth="1"/>
@@ -1317,7 +1403,7 @@
     <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="36" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="10.85546875" bestFit="1" customWidth="1"/>
@@ -1355,20 +1441,22 @@
     <col min="49" max="49" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="14.5703125" customWidth="1"/>
-    <col min="56" max="56" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="17" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="14.5703125" customWidth="1"/>
+    <col min="58" max="58" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="17" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -1523,45 +1611,51 @@
         <v>102</v>
       </c>
       <c r="AZ1" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="BA1" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="BB1" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="BA1" s="24" t="s">
+      <c r="BC1" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="BB1" s="24" t="s">
+      <c r="BD1" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="BC1" s="24" t="s">
+      <c r="BE1" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="BD1" s="24" t="s">
+      <c r="BF1" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="BE1" s="24" t="s">
+      <c r="BG1" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="BF1" s="24" t="s">
+      <c r="BH1" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="BG1" s="24" t="s">
+      <c r="BI1" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="BH1" s="24" t="s">
+      <c r="BJ1" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="BI1" s="24" t="s">
+      <c r="BK1" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="BJ1" s="24" t="s">
+      <c r="BL1" s="24" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:62" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:64" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>59</v>
+        <v>145</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>17</v>
@@ -1591,7 +1685,7 @@
         <v>26</v>
       </c>
       <c r="L2" s="20" t="s">
-        <v>123</v>
+        <v>140</v>
       </c>
       <c r="M2" s="20" t="s">
         <v>47</v>
@@ -1642,10 +1736,10 @@
         <v>56</v>
       </c>
       <c r="AC2" s="26">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="AD2" s="27" t="s">
-        <v>72</v>
+        <v>123</v>
       </c>
       <c r="AE2" s="28" t="s">
         <v>64</v>
@@ -1711,121 +1805,940 @@
         <v>103</v>
       </c>
       <c r="AZ2" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="BA2" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="BB2" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="BA2" s="26" t="s">
+      <c r="BC2" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="BB2" s="26" t="s">
+      <c r="BD2" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="BC2" s="26" t="s">
+      <c r="BE2" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="BD2" s="26" t="s">
+      <c r="BF2" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="BE2" s="26" t="s">
+      <c r="BG2" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="BF2" s="26" t="s">
+      <c r="BH2" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="BG2" s="26" t="s">
+      <c r="BI2" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="BH2" s="26" t="s">
+      <c r="BJ2" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="BI2" s="26" t="s">
+      <c r="BK2" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="BJ2" s="26" t="s">
+      <c r="BL2" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="M3" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="N3" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q3" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="R3" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="S3" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="T3" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="U3" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="V3" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="W3" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="X3" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y3" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z3" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA3" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB3" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC3" s="26">
+        <v>4</v>
+      </c>
+      <c r="AD3" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="AE3" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF3" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG3" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH3" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI3" s="26">
+        <v>1</v>
+      </c>
+      <c r="AJ3" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="AK3" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL3" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="AM3" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="AN3" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="AO3" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="AP3" s="26">
+        <v>1000</v>
+      </c>
+      <c r="AQ3" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="AR3" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="AS3" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="AT3" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="AU3" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="AV3" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="AW3" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="AX3" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="AY3" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="AZ3" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="BA3" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="BB3" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="BC3" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="BD3" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="BE3" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="BF3" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="BG3" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="BH3" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="BI3" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="BJ3" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="BK3" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="BL3" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="M4" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="N4" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="P4" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q4" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="R4" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="S4" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="T4" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="U4" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="V4" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="W4" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="X4" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y4" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z4" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA4" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB4" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC4" s="26">
+        <v>6</v>
+      </c>
+      <c r="AD4" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="AE4" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF4" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG4" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH4" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI4" s="26">
+        <v>1</v>
+      </c>
+      <c r="AJ4" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="AK4" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL4" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="AM4" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="AN4" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="AO4" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="AP4" s="26">
+        <v>1000</v>
+      </c>
+      <c r="AQ4" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="AR4" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="AS4" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="AT4" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="AU4" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="AV4" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="AW4" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="AX4" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="AY4" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="AZ4" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="BA4" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="BB4" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="BC4" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="BD4" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="BE4" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="BF4" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="BG4" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="BH4" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="BI4" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="BJ4" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="BK4" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="BL4" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="M5" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="N5" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="P5" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q5" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="R5" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="S5" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="T5" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="U5" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="V5" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="W5" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="X5" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y5" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z5" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA5" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB5" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC5" s="26">
+        <v>2</v>
+      </c>
+      <c r="AD5" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="AE5" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF5" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG5" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH5" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI5" s="26">
+        <v>1</v>
+      </c>
+      <c r="AJ5" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="AK5" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL5" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="AM5" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="AN5" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="AO5" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="AP5" s="26">
+        <v>1000</v>
+      </c>
+      <c r="AQ5" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="AR5" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="AS5" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="AT5" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="AU5" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="AV5" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="AW5" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="AX5" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="AY5" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="AZ5" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="BA5" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="BB5" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="BC5" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="BD5" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="BE5" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="BF5" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="BG5" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="BH5" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="BI5" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="BJ5" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="BK5" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="BL5" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="M6" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="N6" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="O6" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q6" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="R6" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="S6" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="T6" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="U6" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="V6" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="W6" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="X6" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y6" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z6" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB6" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC6" s="26">
+        <v>3</v>
+      </c>
+      <c r="AD6" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="AE6" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF6" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG6" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH6" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI6" s="26">
+        <v>1</v>
+      </c>
+      <c r="AJ6" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="AK6" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL6" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="AM6" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="AN6" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="AO6" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="AP6" s="26">
+        <v>1000</v>
+      </c>
+      <c r="AQ6" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="AR6" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="AS6" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="AT6" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="AU6" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="AV6" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="AW6" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="AX6" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="AY6" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="AZ6" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="BA6" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="BB6" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="BC6" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="BD6" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="BE6" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="BF6" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="BG6" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="BH6" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="BI6" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="BJ6" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="BK6" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="BL6" s="26" t="s">
         <v>121</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="25">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2 BE2:BF2" xr:uid="{DF4A688D-EAE1-44C4-A7BF-2441206560DF}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2:V6 BG2:BH6" xr:uid="{DF4A688D-EAE1-44C4-A7BF-2441206560DF}">
       <formula1>"One Way,Round Trip"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2" xr:uid="{C1983F1A-F21B-4E83-AC36-25F786ECE188}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U6" xr:uid="{C1983F1A-F21B-4E83-AC36-25F786ECE188}">
       <formula1>"Business trip - QL Business policy,Business trip  - Testing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB2 BA2" xr:uid="{C95F136A-C84B-4EFC-8F0A-C5E05E905915}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB2:AB6 BC2:BC6" xr:uid="{C95F136A-C84B-4EFC-8F0A-C5E05E905915}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2 AF2" xr:uid="{9202FC0C-BCA9-40FB-8FF8-A27DC37B6D25}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2:W6 AF2:AF6" xr:uid="{9202FC0C-BCA9-40FB-8FF8-A27DC37B6D25}">
       <formula1>"Economy,Business,First,Premium Economy"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2" xr:uid="{5E1520F8-7AF4-409C-B5D6-919D7B2BA1F6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T6" xr:uid="{5E1520F8-7AF4-409C-B5D6-919D7B2BA1F6}">
       <formula1>"Domestic,International"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2" xr:uid="{3CF9D7CF-D256-48B2-8FDC-607D2BB763BA}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S6" xr:uid="{3CF9D7CF-D256-48B2-8FDC-607D2BB763BA}">
       <formula1>"Flight,Hotel,MoreProduct"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{6F3754F0-FEB5-4A74-A098-386619C330F2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F6" xr:uid="{6F3754F0-FEB5-4A74-A098-386619C330F2}">
       <formula1>"shekhar.singh@quadlabs.com,sachin.kumar@quadlabs.com,Laxmi.khanal@quadlabs.com,ayushi.shivhare@quadlabs.com,Vikrant.prajapati@quadlabs.com,ankit.singh@quadlabs.com"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2" xr:uid="{B22660F1-1D7B-472C-B385-4498CEB0DA09}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K6" xr:uid="{B22660F1-1D7B-472C-B385-4498CEB0DA09}">
       <formula1>"Laxmi@123,Admin@123,S21FUMK6JAPLBYO,Shubham@123,BAVYBXVY09FKGTY,Piyush@123,Ankur@123,DWUFR8WRAR6SL1M"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{116AEC81-F8D8-4985-98F0-6A7FFCE8C8D8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C6" xr:uid="{116AEC81-F8D8-4985-98F0-6A7FFCE8C8D8}">
       <formula1>"sbt,preprod117"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{60D09136-C750-4680-A34A-320457565344}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I6" xr:uid="{60D09136-C750-4680-A34A-320457565344}">
       <formula1>"Administrator,Travel Arranger,Employee"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{02472E1C-DC1C-4747-98BD-674732B68CC6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H6" xr:uid="{02472E1C-DC1C-4747-98BD-674732B68CC6}">
       <formula1>"Saurabh,Prince Chaurasia,Gunjan Swain,Shubham,Laxmi Khanal,Sudesh Kumar,Piyush,Ankur,D Divaker S,Ankur Yadav,Sachin Kumar"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2" xr:uid="{0C998EC2-A7BD-4826-A679-6CAE65284F8A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J6" xr:uid="{0C998EC2-A7BD-4826-A679-6CAE65284F8A}">
       <formula1>"Shubham1,Shubham,rsudesh15,Saurabh,Laxmi,sachinkumar,Piyush,Ankur"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{27C1FD54-4DE8-44B1-B330-CFC211150764}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E6" xr:uid="{27C1FD54-4DE8-44B1-B330-CFC211150764}">
       <formula1>"//staging117/sbt,//preprod.quadlabs.net/sbt/#,test.quadlabs.net/sbt,tripsource.co.in/sbt/#,//test.quadlabs.net/SSO_Login"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{14BBF75D-F3C0-4D66-9C5B-4BEB838B38A6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D6" xr:uid="{14BBF75D-F3C0-4D66-9C5B-4BEB838B38A6}">
       <formula1>"Normal,SSO"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC2" xr:uid="{222BD394-E544-4494-B737-94D45AE13ED2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC2:AC6" xr:uid="{222BD394-E544-4494-B737-94D45AE13ED2}">
       <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE2" xr:uid="{CAB9BF8E-74B9-4F1A-ADB8-274C852A9C91}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE2:AE6" xr:uid="{CAB9BF8E-74B9-4F1A-ADB8-274C852A9C91}">
       <formula1>"One Way,Round Trip,MultiCity"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI2" xr:uid="{072D0C7B-288B-4876-A047-183510734653}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI2:AI6" xr:uid="{072D0C7B-288B-4876-A047-183510734653}">
       <formula1>"1,2,3,4,5"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO2" xr:uid="{B18970A4-F4BE-4D08-8C98-C9B68EEC4E30}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO2:AO6" xr:uid="{B18970A4-F4BE-4D08-8C98-C9B68EEC4E30}">
       <formula1>"Normal,Luxury"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AV2" xr:uid="{B7702C5C-9F49-4BB5-8E2F-60199DFB5DBC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AV2:AV6" xr:uid="{B7702C5C-9F49-4BB5-8E2F-60199DFB5DBC}">
       <formula1>"Sedan ,SUV,Others"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AW2" xr:uid="{09F39DBE-21FB-423D-9E44-E411BC3E112B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AW2:AW6" xr:uid="{09F39DBE-21FB-423D-9E44-E411BC3E112B}">
       <formula1>"Transfers,Local Use,Outstation,Others "</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AX2" xr:uid="{57AFCA4F-73C7-489F-87D7-3884F385DAFD}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AX2:AX6" xr:uid="{57AFCA4F-73C7-489F-87D7-3884F385DAFD}">
       <formula1>"Bisht Travels [6683],Dilpreet.Singh [VBAll],Shaan_Test_Supplier [Shaan Quadlabs],Hertz Brazil [HZBR],Tourico [TOUR],AMERICAN AIRLINE [0012],MALAYSIA ARLN [232],Ashish [321],Hotel_Supplier [211287],Abacus Travels [555],GDS Travels [4567],Ashu Yadav [S007]"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AY2" xr:uid="{B1F3BC6F-9159-49FB-BC67-7917E01AC80B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AY2:AY6" xr:uid="{B1F3BC6F-9159-49FB-BC67-7917E01AC80B}">
       <formula1>"Visitor,Tourist,Employment,Work Permit,Business,Student,Dependent,Work Permit Dependent,Family Visitor,Domestic Worker,Permanent Migration"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AZ2" xr:uid="{CF313994-AC25-49DA-957E-D0AE3F825E4E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BB2:BB6" xr:uid="{CF313994-AC25-49DA-957E-D0AE3F825E4E}">
       <formula1>"Excluding USA,Including USA"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BI2" xr:uid="{63A68163-1655-4818-AD76-238E7E466689}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BK2:BK6" xr:uid="{63A68163-1655-4818-AD76-238E7E466689}">
       <formula1>"Male,Female,Others"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BJ2" xr:uid="{B4F78EDE-58D7-4E2C-B20C-72BF7B0C5141}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BL2:BL6" xr:uid="{B4F78EDE-58D7-4E2C-B20C-72BF7B0C5141}">
       <formula1>"Voter ID,Passport,PAN Card,Driving License"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="K2" r:id="rId1" display="Admin@123" xr:uid="{2581EA54-2092-4681-AD4E-6F1A6F7272CD}"/>
     <hyperlink ref="F2" r:id="rId2" display="shekhar.singh@quadlabs.com" xr:uid="{E59B4478-6F3E-4D02-B79B-8644A35B9D35}"/>
+    <hyperlink ref="K3" r:id="rId3" display="Admin@123" xr:uid="{B8A8A409-AEFF-4B06-B120-47D9AD3290F9}"/>
+    <hyperlink ref="F3" r:id="rId4" display="shekhar.singh@quadlabs.com" xr:uid="{829631EE-EE5A-4789-B0A5-5ED3C3D1F926}"/>
+    <hyperlink ref="K4" r:id="rId5" display="Admin@123" xr:uid="{2A2490F9-24FA-419C-8F0D-4CCC8E32FDB1}"/>
+    <hyperlink ref="F4" r:id="rId6" display="shekhar.singh@quadlabs.com" xr:uid="{AEBC5550-1E41-41B4-9D47-7027DE223C78}"/>
+    <hyperlink ref="K5" r:id="rId7" display="Admin@123" xr:uid="{E48CAF42-B26F-41F9-8F3C-EB2D15611D15}"/>
+    <hyperlink ref="F5" r:id="rId8" display="shekhar.singh@quadlabs.com" xr:uid="{514A49E2-0EAA-4A82-985C-0A2CBFBCB2C7}"/>
+    <hyperlink ref="K6" r:id="rId9" display="Admin@123" xr:uid="{D2148694-718F-4ADF-AFA3-9BB3788A8760}"/>
+    <hyperlink ref="F6" r:id="rId10" display="shekhar.singh@quadlabs.com" xr:uid="{1FBF36D9-2227-4478-81E8-4B723D96293D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF56EFD0-221F-4050-9307-8353084A0A30}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="94.28515625" style="30" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>